<commit_message>
Migrar OpenCV de carpeta
</commit_message>
<xml_diff>
--- a/Avances.xlsx
+++ b/Avances.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="22Mayo" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t xml:space="preserve">Correcciones </t>
   </si>
@@ -203,9 +204,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -216,6 +214,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -464,6 +465,428 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7499-4D74-8C48-A24FCDF3E0E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1919737119"/>
+        <c:axId val="1919737951"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1919737119"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1919737951"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1919737951"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1919737119"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Comparativa</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-MX" baseline="0"/>
+              <a:t> de lo realizado vs planeado</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'22Mayo'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Progreso %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'22Mayo'!$E$3:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F48F-4589-92B3-5B45696F9DD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'22Mayo'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'22Mayo'!$F$3:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F48F-4589-92B3-5B45696F9DD0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -703,7 +1126,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1225,6 +2191,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>883227</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>31173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>432954</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>107373</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1506,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection sqref="A1:F17"/>
+    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,52 +2524,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>43850</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>80</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1581,156 +2584,156 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="5">
+      <c r="B5" s="1"/>
+      <c r="C5" s="4">
         <v>43857</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>43858</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>100</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>43859</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>43868</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>100</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>43871</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>43882</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>100</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>43885</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>65</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>43900</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>45</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="5">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4">
         <v>43910</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>43906</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>70</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5">
+      <c r="B12" s="1"/>
+      <c r="C12" s="4">
         <v>43921</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1745,72 +2748,72 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="5">
+      <c r="B14" s="1"/>
+      <c r="C14" s="4">
         <v>43922</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>43928</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>55</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="5">
+      <c r="B15" s="1"/>
+      <c r="C15" s="4">
         <v>43928</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>43941</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5">
+      <c r="B16" s="1"/>
+      <c r="C16" s="4">
         <v>43941</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>43946</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5">
+      <c r="B17" s="1"/>
+      <c r="C17" s="4">
         <v>43946</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>43955</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1822,4 +2825,326 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F17" sqref="A1:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>43850</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1">
+        <v>80</v>
+      </c>
+      <c r="F3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4">
+        <v>43857</v>
+      </c>
+      <c r="D5" s="4">
+        <v>43858</v>
+      </c>
+      <c r="E5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4">
+        <v>43859</v>
+      </c>
+      <c r="D6" s="4">
+        <v>43868</v>
+      </c>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43871</v>
+      </c>
+      <c r="D7" s="4">
+        <v>43882</v>
+      </c>
+      <c r="E7" s="1">
+        <v>100</v>
+      </c>
+      <c r="F7" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4">
+        <v>43885</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1">
+        <v>80</v>
+      </c>
+      <c r="F8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4">
+        <v>43900</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1">
+        <v>90</v>
+      </c>
+      <c r="F9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4">
+        <v>43910</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4">
+        <v>43906</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1">
+        <v>70</v>
+      </c>
+      <c r="F11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="4">
+        <v>43921</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="4">
+        <v>43922</v>
+      </c>
+      <c r="D14" s="4">
+        <v>43928</v>
+      </c>
+      <c r="E14" s="1">
+        <v>55</v>
+      </c>
+      <c r="F14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="4">
+        <v>43928</v>
+      </c>
+      <c r="D15" s="4">
+        <v>43941</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="4">
+        <v>43941</v>
+      </c>
+      <c r="D16" s="4">
+        <v>43946</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="4">
+        <v>43946</v>
+      </c>
+      <c r="D17" s="4">
+        <v>43955</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A13:F13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>